<commit_message>
refactor: refactoring information model to better address requirements
</commit_message>
<xml_diff>
--- a/rki.za.vzd/TerminologyManagementSupportingResources/LocationType.xlsx
+++ b/rki.za.vzd/TerminologyManagementSupportingResources/LocationType.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oro/Projekte/EMIGA/Informationsmodell/github/rki.za.vzd/rki.za.vzd/TerminologyManagementSupportingResources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FBB3C0-61AA-1945-AAE2-09E7AFD0700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981A4071-6DBD-0546-B99F-0AFD2BB8763D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="1380" windowWidth="49880" windowHeight="29680" xr2:uid="{71C88F08-19D8-445E-B2A1-D2A7FD9C7971}"/>
   </bookViews>
@@ -208,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -232,7 +232,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -580,7 +579,7 @@
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>